<commit_message>
IACET_Dispatcher folder added and in this folder read mail and check attachment workflow added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\UiPath\IACET\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441CB9A8-4EF3-4BB5-AF6F-328B495470BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,30 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>FolderName</t>
+  </si>
+  <si>
+    <t>Inbox</t>
+  </si>
+  <si>
+    <t>ProjectSubjectFolder</t>
+  </si>
+  <si>
+    <t>IACET</t>
+  </si>
+  <si>
+    <t>OtherSubjectFolder</t>
+  </si>
+  <si>
+    <t>Other mails</t>
+  </si>
+  <si>
+    <t>ProjectSubject</t>
+  </si>
+  <si>
+    <t>IACET client Details</t>
   </si>
 </sst>
 </file>
@@ -212,10 +236,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,16 +561,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,7 +618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +628,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -615,10 +639,38 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1623,12 +1675,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1717,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1728,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1842,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2782,14 +2834,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Save Attachment worklflow created
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\AppData\Local\Programs\UiPath\Studio\IACET\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77657F90-4F94-4115-84BA-36781487D766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D971B9DC-83B7-4BCE-80E8-41301A7FF6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -171,13 +171,19 @@
     <t>khan.firoz92n@outlook.com</t>
   </si>
   <si>
-    <t>Folder</t>
-  </si>
-  <si>
     <t>Top_Email</t>
   </si>
   <si>
     <t>MailRead_Folder</t>
+  </si>
+  <si>
+    <t>Mail_Folder</t>
+  </si>
+  <si>
+    <t>SaveEmail_FileFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\admin\AppData\Local\Programs\UiPath\Studio\IACET\Save Email Attachment</t>
   </si>
 </sst>
 </file>
@@ -559,7 +565,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -650,7 +656,7 @@
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>45</v>
@@ -659,23 +665,30 @@
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="5">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Split PDF Workflow created
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\AppData\Local\Programs\UiPath\Studio\IACET\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D971B9DC-83B7-4BCE-80E8-41301A7FF6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B5DE2E-D115-4BD1-9D41-FACA951CB057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -180,10 +180,28 @@
     <t>Mail_Folder</t>
   </si>
   <si>
-    <t>SaveEmail_FileFolder</t>
-  </si>
-  <si>
     <t>C:\Users\admin\AppData\Local\Programs\UiPath\Studio\IACET\Save Email Attachment</t>
+  </si>
+  <si>
+    <t>Save Email Attachment</t>
+  </si>
+  <si>
+    <t>IACET_Client_Details</t>
+  </si>
+  <si>
+    <t>IACET client Details[2305843009213758970].pdf</t>
+  </si>
+  <si>
+    <t>OutputFolder1</t>
+  </si>
+  <si>
+    <t>OutputFolder2</t>
+  </si>
+  <si>
+    <t>C:\Users\admin\AppData\Local\Programs\UiPath\Studio\IACET\Data\OutputFolder1</t>
+  </si>
+  <si>
+    <t>C:\Users\admin\AppData\Local\Programs\UiPath\Studio\IACET\Data\OutputFolder2</t>
   </si>
 </sst>
 </file>
@@ -564,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -683,29 +701,50 @@
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
         <v>51</v>
       </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>